<commit_message>
Giải thích tưs hóa
</commit_message>
<xml_diff>
--- a/LuanQuanLoc.xlsx
+++ b/LuanQuanLoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA8EEA7-5599-40CB-8222-7A9E11873F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0234145-8016-47CF-BC14-0854008EB84D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3927" uniqueCount="2213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3944" uniqueCount="2226">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -6699,6 +6699,45 @@
   </si>
   <si>
     <t>Liên quan tới phạm pháp, có thể không ngồi cùng nhưng cũng sẽ tốn kém tiền bạc.</t>
+  </si>
+  <si>
+    <t>Văn Xương, Hóa Kỵ đồng cung tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Văn xương chủ về công danh, khoa giáp, về văn bút, danh dự, hóa kỵ thì thi cử không đỗ, văn bút bị tổn hại, công danh sa sút, thanh danh bị hoen ố.</t>
+  </si>
+  <si>
+    <t>Vì nhầm lẫn giấy tờ hoặc là vì lo giấy tờ cho người khác, bảo lãnh cho người khác, hoặc vì nợ nần mà xảy ra nhiều chuyện dẫn đến sự nghiệp gặp nhiều sóng gió.</t>
+  </si>
+  <si>
+    <t>Không nên đánh bài bạc, không nên đầu cơ. Nên tuân thủ luật pháp, không nên cố tình trốn thuế.</t>
+  </si>
+  <si>
+    <t>Văn Khúc, Hóa Kỵ đồng cung tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Cơ đồng cung với Hóa Kỵ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên cơ là sao tăng thọ, trí tuệ, nếu Hóa kỵ thì trí tuệ sa sút mà dẫn đến nhiều sai lầm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thiên Lương đồng cung với Địa Kiếp, Địa Không tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Mọi chuyện khó thành, nên tu tâm cửa Phật</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Thiên Lương đồng cung ở Quan Lộc gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Thiên Cơ, Hóa Kỵ đồng cung ở Quan Lộc gặp các sao Kình Dương, Đà La, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tâm tình không được tốt, dễ bị thương bên ngoài, hoặc là mất ngủ.</t>
+  </si>
+  <si>
+    <t>Cuộc đời sự nghiệp luôn biến động, hơn nữa càng biến động thì càng xấu. Một đời như bèo dạt theo sóng nước, rất kỵ đầu cơ nếu không có thể phá sản.</t>
   </si>
 </sst>
 </file>
@@ -7089,10 +7128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G1958"/>
+  <dimension ref="A2:G1964"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1950" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1961" sqref="C1961"/>
+    <sheetView tabSelected="1" topLeftCell="A1956" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1964" sqref="C1964"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22809,7 +22848,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="1953" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1953" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1953" s="1" t="s">
         <v>2201</v>
       </c>
@@ -22817,7 +22856,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="1954" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1954" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1954" s="1" t="s">
         <v>2203</v>
       </c>
@@ -22825,7 +22864,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="1955" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1955" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1955" s="1" t="s">
         <v>2205</v>
       </c>
@@ -22833,7 +22872,7 @@
         <v>2206</v>
       </c>
     </row>
-    <row r="1956" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1956" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1956" s="1" t="s">
         <v>2207</v>
       </c>
@@ -22841,7 +22880,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="1957" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1957" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1957" s="1" t="s">
         <v>2209</v>
       </c>
@@ -22849,18 +22888,81 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="1958" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1958" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1958" s="1" t="s">
         <v>2211</v>
       </c>
       <c r="B1958" s="1" t="s">
         <v>2212</v>
+      </c>
+    </row>
+    <row r="1959" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1959" s="1" t="s">
+        <v>2213</v>
+      </c>
+      <c r="B1959" s="1" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C1959" s="1" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D1959" s="1" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="1960" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1960" s="1" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B1960" s="1" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C1960" s="1" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D1960" s="1" t="s">
+        <v>2216</v>
+      </c>
+    </row>
+    <row r="1961" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1961" s="1" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B1961" s="1" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="1962" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1962" s="1" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B1962" s="1" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="1963" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1963" s="1" t="s">
+        <v>2222</v>
+      </c>
+      <c r="B1963" s="1" t="s">
+        <v>2221</v>
+      </c>
+    </row>
+    <row r="1964" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1964" s="1" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B1964" s="1" t="s">
+        <v>2224</v>
+      </c>
+      <c r="C1964" s="1" t="s">
+        <v>2225</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:E1956" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A62:B1950 A1958:B1048576 A1951:A1957 A61 A1:B55 A57:B60 A56">
+  <conditionalFormatting sqref="A62:B1950 A1951:A1957 A61 A1:B55 A57:B60 A56 A1958:B1048576">
     <cfRule type="duplicateValues" dxfId="5" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1945:B1949">

</xml_diff>